<commit_message>
Atualização automática de TRES_COROAS.xlsx
</commit_message>
<xml_diff>
--- a/TRES_COROAS.xlsx
+++ b/TRES_COROAS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DC1CF48B-FF44-4043-947D-4168C0D8CCA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A4ACC609-85D1-4680-B883-9A33DDDE9572}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1172,7 +1172,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{833B3B62-DD5F-442F-957A-C5E46DA70B16}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{FDE13714-A885-4000-90F5-2F88B8C8673D}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1202,10 +1202,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BDA31C51-23BF-44D1-BE66-0025D44542DF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6A76495-039E-4A31-A983-0682764AB785}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1243,7 +1243,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52D66041-2A9A-4A54-9886-26EEE28E503F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E80AF110-189B-4C00-B1B5-36D69B20CC35}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1306,7 +1306,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C626F998-EE05-44CE-9145-51DF4C88674B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0380693-35DE-489E-BCC8-D411455D7CA3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1325,7 +1325,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF305D9A-61F1-A955-E8F5-7EC1ED2AFDB0}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D9817D9-9120-9D69-63EF-829CC954440E}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1374,7 +1374,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E3558B4-8756-C3AF-3AD6-276BC0AC62C3}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{027B24E7-005D-8412-6C62-998ABA60F3F5}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1393,7 +1393,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8BAC2462-C8A3-9B3E-A376-74C824770128}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4805961A-5E69-5F0D-03BB-F92DE317BC8B}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1424,7 +1424,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F57187D-0EFD-085D-AC6B-37981450DABC}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{984CBE57-E0B7-317C-2AB5-14629BC19627}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1455,7 +1455,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A0F28AB-178F-659E-A057-66D5474E1ADF}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5234167-658B-AACE-7284-6FB2663A015E}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1498,7 +1498,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC45CD87-ACAF-4FC7-911D-BA407A9DDF27}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E69028B-5A2E-4C35-B37E-358595A0E0FA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1536,7 +1536,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F62917A1-3A41-420A-93E6-3530F537762C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74FC1C36-0F2E-4F0A-818D-EE2ED9BF09E5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1579,7 +1579,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6E1F572-98CF-4F6C-B6EF-6994E30CB791}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42E90989-0258-4FF7-9ACB-095D6149260E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1892,7 +1892,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DFA437E-4E0E-432B-821B-4AB27F19B77A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCE9C710-D844-4301-8AE8-C06395D97F7A}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>